<commit_message>
Remove the configuration.ini via gitignore
</commit_message>
<xml_diff>
--- a/stg_data.xlsx
+++ b/stg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antho/Documents/Job Search - 2023/Port-Proj/SeatMe_ETL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A658674-0874-1F42-811F-3824BFEB6CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E753CA-41B4-BE46-B45A-1A6AEE8E733E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="16500" windowHeight="18400" activeTab="2" xr2:uid="{EF7C40AC-D27A-1C41-AF97-0262E461BD55}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="11520" windowHeight="18400" activeTab="2" xr2:uid="{EF7C40AC-D27A-1C41-AF97-0262E461BD55}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="148">
   <si>
     <t>email</t>
   </si>
@@ -467,13 +467,28 @@
   </si>
   <si>
     <t>American</t>
+  </si>
+  <si>
+    <t> (718) 349-0011</t>
+  </si>
+  <si>
+    <t>Southern Asian</t>
+  </si>
+  <si>
+    <t>614 Manhattan Ave, Brooklyn, NY 11222</t>
+  </si>
+  <si>
+    <t>Baoburg</t>
+  </si>
+  <si>
+    <t>332 Driggs Ave, Brooklyn, New York, 11222</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -488,6 +503,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFBDC1C6"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -511,10 +532,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1942,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29AF127-E79D-8249-BB8E-1FFB216F50BB}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2023,6 +2045,9 @@
       <c r="C3" t="s">
         <v>142</v>
       </c>
+      <c r="D3" t="s">
+        <v>147</v>
+      </c>
       <c r="E3">
         <v>20</v>
       </c>
@@ -2032,13 +2057,43 @@
       <c r="H3">
         <v>25</v>
       </c>
+      <c r="I3">
+        <v>69</v>
+      </c>
       <c r="J3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J4" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.google.com/search?q=oxomoco+brooklyn+phone+number&amp;sca_esv=584304970&amp;sxsrf=AM9HkKlXzFxv2PAcviHChWCnZKgGXRn-IQ%3A1700579201143&amp;ei=gcdcZdGeCJSt5NoP5pq7-A8&amp;ved=0ahUKEwiR48iZr9WCAxWUFlkFHWbNDv8Q4dUDCBE&amp;uact=5&amp;oq=oxomoco+brooklyn+phone+number&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiHW94b21vY28gYnJvb2tseW4gcGhvbmUgbnVtYmVyMgUQIRigATIFECEYqwJIoBRQ8gVYrBNwAXgBkAEAmAGFAaABwQqqAQM3Lja4AQPIAQD4AQHCAgoQABhHGNYEGLADwgIZEC4YgAQYigUYxwEYrwEYyAMYsAMYQ9gBAcICCxAuGIAEGMcBGK8BwgIKEAAYgAQYigUYQ8ICBhAAGBYYHsICAhAmwgILEAAYgAQYigUYhgPCAhoQLhiABBjHARivARiXBRjcBBjeBBjgBNgBAsICCBAhGBYYHhgd4gMEGAAgQYgGAZAGDLoGBAgBGAi6BgYIAhABGBQ&amp;sclient=gws-wiz-serp" xr:uid="{F6E3531D-F972-B743-ADEA-C51DB6D32C2D}"/>
+    <hyperlink ref="I4" r:id="rId2" display="https://www.google.com/search?q=baoberg&amp;oq=baoberg&amp;gs_lcrp=EgZjaHJvbWUyBggAEEUYOTIPCAEQLhgKGK8BGMcBGIAEMgkIAhAAGAoYgAQyCQgDEAAYChiABDIJCAQQABgKGIAEMgkIBRAAGAoYgAQyCQgGEAAYChiABDIMCAcQABgFGAoYDxge0gEIMTY5MGowajSoAgCwAgA&amp;sourceid=chrome&amp;ie=UTF-8" xr:uid="{81D3B009-C100-DE44-8204-D67AC5AA63B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>